<commit_message>
results for straight line lipschitz error computation
</commit_message>
<xml_diff>
--- a/graphs/lipschitz_results.xlsx
+++ b/graphs/lipschitz_results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
   <si>
     <t>Jet Engine</t>
   </si>
@@ -269,20 +269,43 @@
     <t>verhulstStar</t>
   </si>
   <si>
-    <t>infinity norm, time in sec</t>
-  </si>
-  <si>
-    <t>component-wise time</t>
-  </si>
-  <si>
     <t>component-wise</t>
+  </si>
+  <si>
+    <t>jetEngine</t>
+  </si>
+  <si>
+    <t>jetEngineStar</t>
+  </si>
+  <si>
+    <t>predatorPreyStar</t>
+  </si>
+  <si>
+    <t>infinity norm, 
+time (sec)</t>
+  </si>
+  <si>
+    <t>component-wise
+ time (sec)</t>
+  </si>
+  <si>
+    <t>diff 
+(this - AA)</t>
+  </si>
+  <si>
+    <t>diff
+(this - AA)</t>
+  </si>
+  <si>
+    <t>diff
+(component - inf)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,6 +353,11 @@
       <color theme="0" tint="-0.14999847407452621"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -340,13 +368,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +388,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -380,8 +408,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -392,16 +460,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -410,16 +472,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -429,6 +504,26 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -438,6 +533,26 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -786,39 +901,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21" style="7" customWidth="1"/>
-    <col min="2" max="3" width="17.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="21" style="6" customWidth="1"/>
+    <col min="2" max="3" width="17.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="6" customWidth="1"/>
     <col min="10" max="10" width="25.1640625" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="36.83203125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="36.83203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="18">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="J2" s="5" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="J2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="36">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -833,21 +948,21 @@
       <c r="K3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>2.1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>1.8</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>38</v>
       </c>
       <c r="G5">
@@ -864,16 +979,16 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>0.33500000000000002</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>16.7</v>
       </c>
       <c r="G7">
@@ -888,24 +1003,24 @@
       <c r="K7" s="1">
         <v>3.9419999999999998E-15</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>0.48</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>0.44</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>37</v>
       </c>
       <c r="G9">
@@ -916,16 +1031,16 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>82</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>7.3</v>
       </c>
       <c r="G11">
@@ -934,29 +1049,29 @@
       <c r="H11">
         <v>0.98853000000000002</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>66.7</v>
       </c>
       <c r="G15">
@@ -967,35 +1082,35 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>5.4</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>11.91</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G21">
@@ -1004,21 +1119,21 @@
       <c r="J21" s="1">
         <v>2.7300000000000002E-15</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="L21" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>8.52</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>22.4</v>
       </c>
       <c r="G23">
@@ -1042,31 +1157,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O27"/>
+  <dimension ref="A2:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5" style="11" customWidth="1"/>
+    <col min="3" max="3" width="5" style="9" customWidth="1"/>
     <col min="4" max="4" width="27" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="2"/>
-    <col min="7" max="7" width="5.6640625" style="11" customWidth="1"/>
-    <col min="8" max="15" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="30.1640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" style="2" customWidth="1"/>
+    <col min="12" max="15" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:15">
+      <c r="D2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="30">
       <c r="A3" s="2" t="s">
         <v>54</v>
       </c>
@@ -1076,713 +1195,804 @@
       <c r="D3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18">
-      <c r="A4" s="9" t="s">
+      <c r="I3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18">
+      <c r="A4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <v>4.6347106030860903E-8</v>
       </c>
-      <c r="C4" s="12">
-        <f>B4-D4</f>
-        <v>-291.82212199632789</v>
-      </c>
+      <c r="C4" s="15"/>
       <c r="D4" s="2">
         <v>291.82212204267501</v>
       </c>
-      <c r="E4" s="2">
-        <v>31.238</v>
-      </c>
-      <c r="G4" s="14">
-        <f>B4-H4</f>
-        <v>4.190834017589055E-8</v>
-      </c>
-      <c r="H4" s="10">
-        <v>4.4387658549703503E-9</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="2">
-        <v>31.742999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18">
-      <c r="A5" s="9" t="s">
+      <c r="F4" s="8">
+        <f>D4-B4</f>
+        <v>291.82212199632789</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="8">
+        <v>2.4391675624488901E-8</v>
+      </c>
+      <c r="I4" s="8">
+        <f>H4-B4</f>
+        <v>-2.1955430406372002E-8</v>
+      </c>
+      <c r="K4" s="17">
+        <f>H4-D4</f>
+        <v>-291.82212201828332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18">
+      <c r="A5" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="2">
         <v>2114297.8359521399</v>
       </c>
-      <c r="C5" s="12">
-        <f t="shared" ref="C5:C27" si="0">B5-D5</f>
-        <v>-375497885702.16406</v>
-      </c>
+      <c r="C5" s="15"/>
       <c r="D5" s="2">
         <v>375500000000</v>
       </c>
-      <c r="E5" s="2">
-        <v>31.283000000000001</v>
-      </c>
-      <c r="G5" s="14">
-        <f t="shared" ref="G5:G27" si="1">B5-H5</f>
-        <v>1937755.445447847</v>
-      </c>
+      <c r="F5" s="8">
+        <f t="shared" ref="F5:F30" si="0">D5-B5</f>
+        <v>375497885702.16406</v>
+      </c>
+      <c r="G5" s="14"/>
       <c r="H5" s="2">
-        <v>176542.390504293</v>
-      </c>
-      <c r="J5" s="2">
-        <v>31.64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18">
-      <c r="A6" s="9" t="s">
+        <v>176542.39050431299</v>
+      </c>
+      <c r="I5" s="8">
+        <f t="shared" ref="I5:I30" si="1">H5-B5</f>
+        <v>-1937755.445447827</v>
+      </c>
+      <c r="K5" s="17">
+        <f t="shared" ref="K5:K30" si="2">H5-D5</f>
+        <v>-375499823457.6095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18">
+      <c r="A6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>4.91905140346289E-13</v>
       </c>
-      <c r="C6" s="12">
-        <f t="shared" si="0"/>
-        <v>-7.0768661270729107E-12</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="C6" s="15"/>
+      <c r="D6" s="8">
         <v>7.5687712674192001E-12</v>
       </c>
-      <c r="E6" s="2">
-        <v>51.408000000000001</v>
-      </c>
-      <c r="G6" s="14">
-        <f t="shared" si="1"/>
-        <v>4.3672151132839529E-13</v>
-      </c>
-      <c r="H6" s="10">
-        <v>5.5183629017893701E-14</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="2">
-        <v>50.472999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="18">
-      <c r="A7" s="9" t="s">
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>7.0768661270729107E-12</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="8">
+        <v>4.8247373575872301E-13</v>
+      </c>
+      <c r="I6" s="8">
+        <f t="shared" si="1"/>
+        <v>-9.431404587565984E-15</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" si="2"/>
+        <v>-7.0862975316604769E-12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18">
+      <c r="A7" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>2.3547845323688901E-6</v>
       </c>
-      <c r="C7" s="12">
-        <f t="shared" si="0"/>
-        <v>-8.6145308433166993E-7</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C7" s="15"/>
+      <c r="D7" s="8">
         <v>3.2162376167005601E-6</v>
       </c>
-      <c r="E7" s="2">
-        <v>49.540999999999997</v>
-      </c>
-      <c r="G7" s="14">
-        <f t="shared" si="1"/>
-        <v>1.2774009274335702E-6</v>
-      </c>
-      <c r="H7" s="10">
-        <v>1.0773836049353199E-6</v>
-      </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="2">
-        <v>50.322000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="18">
-      <c r="A8" s="9" t="s">
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>8.6145308433166993E-7</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="8">
+        <v>1.0773840322254299E-6</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.2774005001434602E-6</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" si="2"/>
+        <v>-2.1388535844751302E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18">
+      <c r="A8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>1.2850339484026499E-12</v>
       </c>
-      <c r="C8" s="12">
-        <f t="shared" si="0"/>
-        <v>-2.2503814401086548E-11</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="C8" s="15"/>
+      <c r="D8" s="8">
         <v>2.3788848349489198E-11</v>
       </c>
-      <c r="E8" s="2">
-        <v>43.064999999999998</v>
-      </c>
-      <c r="G8" s="14">
-        <f t="shared" si="1"/>
-        <v>1.1337945196788169E-12</v>
-      </c>
-      <c r="H8" s="10">
-        <v>1.5123942872383299E-13</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="2">
-        <v>43.256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="18">
-      <c r="A9" s="9" t="s">
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>2.2503814401086548E-11</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="8">
+        <v>1.2582571520286501E-12</v>
+      </c>
+      <c r="I8" s="8">
+        <f t="shared" si="1"/>
+        <v>-2.6776796373999848E-14</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" si="2"/>
+        <v>-2.253059119746055E-11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18">
+      <c r="A9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>6.2018464551160697E-5</v>
       </c>
-      <c r="C9" s="12">
-        <f t="shared" si="0"/>
-        <v>-8.1099722530490592E-3</v>
-      </c>
+      <c r="C9" s="15"/>
       <c r="D9" s="2">
         <v>8.1719907176002193E-3</v>
       </c>
-      <c r="E9" s="2">
-        <v>43.100999999999999</v>
-      </c>
-      <c r="G9" s="14">
-        <f t="shared" si="1"/>
-        <v>3.4486453979393501E-5</v>
-      </c>
-      <c r="H9" s="10">
-        <v>2.75320105717672E-5</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="2">
-        <v>43.121000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18">
-      <c r="A10" s="9" t="s">
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>8.1099722530490592E-3</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="8">
+        <v>2.7532011678784899E-5</v>
+      </c>
+      <c r="I9" s="8">
+        <f t="shared" si="1"/>
+        <v>-3.4486452872375798E-5</v>
+      </c>
+      <c r="K9" s="17">
+        <f t="shared" si="2"/>
+        <v>-8.1444587059214344E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18">
+      <c r="A10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>2.0274450741076099E-13</v>
       </c>
-      <c r="C10" s="12">
-        <f t="shared" si="0"/>
-        <v>-1.3481518328952791E-12</v>
-      </c>
-      <c r="D10" s="10">
+      <c r="C10" s="15"/>
+      <c r="D10" s="8">
         <v>1.5508963403060401E-12</v>
       </c>
-      <c r="E10" s="2">
-        <v>81.703000000000003</v>
-      </c>
-      <c r="G10" s="14">
-        <f t="shared" si="1"/>
-        <v>1.8424641315316178E-13</v>
-      </c>
-      <c r="H10" s="10">
-        <v>1.8498094257599199E-14</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="2">
-        <v>81.816999999999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="18">
-      <c r="A11" s="9" t="s">
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3481518328952791E-12</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="8">
+        <v>1.89817199412561E-13</v>
+      </c>
+      <c r="I10" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.292730799819999E-14</v>
+      </c>
+      <c r="K10" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.361079140893479E-12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18">
+      <c r="A11" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="2">
         <v>1.22779091632187E-4</v>
       </c>
-      <c r="C11" s="13">
-        <f t="shared" si="0"/>
-        <v>6.1566642966727603E-5</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="C11" s="15"/>
+      <c r="D11" s="8">
         <v>6.1212448665459395E-5</v>
       </c>
-      <c r="E11" s="2">
-        <v>89.501000000000005</v>
-      </c>
-      <c r="G11" s="14">
-        <f t="shared" si="1"/>
-        <v>6.1525522358431999E-5</v>
-      </c>
-      <c r="H11" s="10">
-        <v>6.1253569273754998E-5</v>
-      </c>
-      <c r="J11" s="2">
-        <v>81.302000000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="18">
-      <c r="A12" s="9" t="s">
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>-6.1566642966727603E-5</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="8">
+        <v>6.1253569445074093E-5</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" si="1"/>
+        <v>-6.1525522187112904E-5</v>
+      </c>
+      <c r="K11" s="18">
+        <f t="shared" si="2"/>
+        <v>4.112077961469817E-8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="18">
+      <c r="A12" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1.61703982148642E-8</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="8">
+        <v>8.5601678323450507E-9</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>-7.6102303825191497E-9</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="8">
+        <v>8.4020009457114102E-9</v>
+      </c>
+      <c r="I12" s="8">
+        <f t="shared" si="1"/>
+        <v>-7.7683972691527903E-9</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.5816688663364052E-10</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" ht="18">
+      <c r="A13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.14001733998549501</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="2">
+        <v>9.5335648310577699E-4</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.13906398350238924</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="2">
+        <v>9.5604725233654599E-4</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" si="1"/>
+        <v>-0.13906129273315845</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="18">
+        <f t="shared" si="2"/>
+        <v>2.6907692307689968E-6</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" ht="18">
+      <c r="A14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B14" s="8">
         <v>2.93531236761047E-16</v>
       </c>
-      <c r="C12" s="12">
-        <f t="shared" si="0"/>
-        <v>-9.2254803535027291E-16</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="C14" s="15"/>
+      <c r="D14" s="8">
         <v>1.2160792721113199E-15</v>
       </c>
-      <c r="E12" s="2">
-        <v>64.322999999999993</v>
-      </c>
-      <c r="G12" s="14">
-        <f t="shared" si="1"/>
-        <v>1.66931989180831E-16</v>
-      </c>
-      <c r="H12" s="10">
-        <v>1.26599247580216E-16</v>
-      </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="2">
-        <v>64.114000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="18">
-      <c r="A13" s="9" t="s">
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>9.2254803535027291E-16</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="8">
+        <v>2.9395681973922702E-16</v>
+      </c>
+      <c r="I14" s="16">
+        <f t="shared" si="1"/>
+        <v>4.2558297818001423E-19</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="2"/>
+        <v>-9.2212245237209294E-16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="18">
+      <c r="A15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="8">
+        <v>9.21678116374064E-5</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="2">
+        <v>2.3615113285604598E-3</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>2.2693435169230535E-3</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="8">
+        <v>9.7853112216226301E-5</v>
+      </c>
+      <c r="I15" s="16">
+        <f t="shared" si="1"/>
+        <v>5.6853005788199014E-6</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="17">
+        <f t="shared" si="2"/>
+        <v>-2.2636582163442333E-3</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" ht="18">
+      <c r="A16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B16" s="8">
         <v>5.0792705700022197E-13</v>
       </c>
-      <c r="C13" s="13">
-        <f t="shared" si="0"/>
-        <v>7.8270725353138967E-14</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="C16" s="15"/>
+      <c r="D16" s="8">
         <v>4.2965633164708301E-13</v>
       </c>
-      <c r="E13" s="2">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="G13" s="14">
-        <f t="shared" si="1"/>
-        <v>3.5471627960195098E-13</v>
-      </c>
-      <c r="H13" s="10">
-        <v>1.53210777398271E-13</v>
-      </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="2">
-        <v>0.26700000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="18">
-      <c r="A14" s="9" t="s">
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>-7.8270725353138967E-14</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="8">
+        <v>5.07927054883157E-13</v>
+      </c>
+      <c r="I16" s="8">
+        <f t="shared" si="1"/>
+        <v>-2.1170649763561217E-21</v>
+      </c>
+      <c r="K16" s="18">
+        <f t="shared" si="2"/>
+        <v>7.827072323607399E-14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="18">
+      <c r="A17" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B17" s="8">
         <v>9.2000035501627902E-7</v>
       </c>
-      <c r="C14" s="13">
-        <f t="shared" si="0"/>
-        <v>4.7000000030000202E-7</v>
-      </c>
-      <c r="D14" s="10">
+      <c r="C17" s="15"/>
+      <c r="D17" s="8">
         <v>4.5000035471627699E-7</v>
       </c>
-      <c r="E14" s="2">
-        <v>0.224</v>
-      </c>
-      <c r="G14" s="14">
-        <f t="shared" si="1"/>
-        <v>3.5501627903754501E-13</v>
-      </c>
-      <c r="H14" s="10">
-        <v>9.1999999999999998E-7</v>
-      </c>
-      <c r="I14" s="10"/>
-      <c r="J14" s="2">
-        <v>0.23499999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="18">
-      <c r="A15" s="9" t="s">
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>-4.7000000030000202E-7</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="8">
+        <v>9.2000035471627699E-7</v>
+      </c>
+      <c r="I17" s="8">
+        <f t="shared" si="1"/>
+        <v>-3.0000202337940969E-16</v>
+      </c>
+      <c r="K17" s="18">
+        <f t="shared" si="2"/>
+        <v>4.7E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="18">
+      <c r="A18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B18" s="8">
         <v>6.4751830685015296E-11</v>
       </c>
-      <c r="C15" s="13">
-        <f t="shared" si="0"/>
-        <v>1.3039569878018995E-11</v>
-      </c>
-      <c r="D15" s="10">
+      <c r="C18" s="15"/>
+      <c r="D18" s="8">
         <v>5.1712260806996301E-11</v>
       </c>
-      <c r="E15" s="2">
-        <v>16.41</v>
-      </c>
-      <c r="G15" s="14">
-        <f t="shared" si="1"/>
-        <v>3.9720187260304295E-11</v>
-      </c>
-      <c r="H15" s="10">
-        <v>2.5031643424711001E-11</v>
-      </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="2">
-        <v>16.664999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="18">
-      <c r="A16" s="9" t="s">
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.3039569878018995E-11</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="8">
+        <v>6.4751830231218804E-11</v>
+      </c>
+      <c r="I18" s="8">
+        <f t="shared" si="1"/>
+        <v>-4.5379649269951065E-19</v>
+      </c>
+      <c r="K18" s="18">
+        <f t="shared" si="2"/>
+        <v>1.3039569424222502E-11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="18">
+      <c r="A19" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B19" s="2">
         <v>1.50310039864787E-4</v>
       </c>
-      <c r="C16" s="13">
-        <f t="shared" si="0"/>
-        <v>7.8300000144600199E-5</v>
-      </c>
-      <c r="D16" s="10">
+      <c r="C19" s="15"/>
+      <c r="D19" s="8">
         <v>7.2010039720186799E-5</v>
       </c>
-      <c r="E16" s="2">
-        <v>16.405999999999999</v>
-      </c>
-      <c r="G16" s="14">
-        <f t="shared" si="1"/>
-        <v>3.9864787008568256E-11</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1.5030999999999999E-4</v>
-      </c>
-      <c r="J16" s="2">
-        <v>16.216000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="18">
-      <c r="A17" s="9" t="s">
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>-7.8300000144600199E-5</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="2">
+        <v>1.5031003972018601E-4</v>
+      </c>
+      <c r="I19" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.4460099242129265E-13</v>
+      </c>
+      <c r="K19" s="18">
+        <f t="shared" si="2"/>
+        <v>7.8299999999999206E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18">
+      <c r="A20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B20" s="8">
         <v>9.5541167016934297E-16</v>
       </c>
-      <c r="C17" s="13">
-        <f t="shared" si="0"/>
-        <v>1.90789812033849E-16</v>
-      </c>
-      <c r="D17" s="10">
+      <c r="C20" s="15"/>
+      <c r="D20" s="8">
         <v>7.6462185813549397E-16</v>
       </c>
-      <c r="E17" s="2">
-        <v>8.83</v>
-      </c>
-      <c r="G17" s="14">
-        <f t="shared" si="1"/>
-        <v>7.8101824526048201E-16</v>
-      </c>
-      <c r="H17" s="10">
-        <v>1.7439342490886101E-16</v>
-      </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="2">
-        <v>8.766</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="18">
-      <c r="A18" s="9" t="s">
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.90789812033849E-16</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="8">
+        <v>7.6462185813549397E-16</v>
+      </c>
+      <c r="I20" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.90789812033849E-16</v>
+      </c>
+      <c r="K20" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="18">
+      <c r="A21" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B21" s="8">
         <v>1.1079985983775101E-15</v>
       </c>
-      <c r="C18" s="13">
-        <f t="shared" si="0"/>
-        <v>2.2916093533810804E-16</v>
-      </c>
-      <c r="D18" s="10">
+      <c r="C21" s="15"/>
+      <c r="D21" s="8">
         <v>8.7883766303940201E-16</v>
       </c>
-      <c r="E18" s="2">
-        <v>1.19</v>
-      </c>
-      <c r="G18" s="14">
-        <f t="shared" si="1"/>
-        <v>8.959616196132761E-16</v>
-      </c>
-      <c r="H18" s="10">
-        <v>2.12036978764234E-16</v>
-      </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="2">
-        <v>1.1990000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="18">
-      <c r="A19" s="9" t="s">
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>-2.2916093533810804E-16</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="8">
+        <v>8.7883766303940201E-16</v>
+      </c>
+      <c r="I21" s="8">
+        <f t="shared" si="1"/>
+        <v>-2.2916093533810804E-16</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="18">
+      <c r="A22" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B22" s="8">
         <v>8.4047352454551996E-16</v>
       </c>
-      <c r="C19" s="13">
-        <f t="shared" si="0"/>
-        <v>2.9490299125532952E-17</v>
-      </c>
-      <c r="D19" s="10">
+      <c r="C22" s="15"/>
+      <c r="D22" s="8">
         <v>8.1098322541998701E-16</v>
       </c>
-      <c r="E19" s="2">
-        <v>2.1389999999999998</v>
-      </c>
-      <c r="G19" s="14">
-        <f t="shared" si="1"/>
-        <v>7.8496237331183875E-16</v>
-      </c>
-      <c r="H19" s="10">
-        <v>5.5511151233681195E-17</v>
-      </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="2">
-        <v>2.1230000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="18">
-      <c r="A20" s="9" t="s">
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>-2.9490299125532952E-17</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="8">
+        <v>8.1098322541998701E-16</v>
+      </c>
+      <c r="I22" s="8">
+        <f t="shared" si="1"/>
+        <v>-2.9490299125532952E-17</v>
+      </c>
+      <c r="K22" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="18">
+      <c r="A23" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B23" s="8">
         <v>1.2416195497345899E-13</v>
       </c>
-      <c r="C20" s="13">
-        <f t="shared" si="0"/>
-        <v>1.6077133509280988E-14</v>
-      </c>
-      <c r="D20" s="10">
+      <c r="C23" s="15"/>
+      <c r="D23" s="8">
         <v>1.08084821464178E-13</v>
       </c>
-      <c r="E20" s="2">
-        <v>25.155000000000001</v>
-      </c>
-      <c r="G20" s="14">
-        <f t="shared" si="1"/>
-        <v>1.1475807216545493E-13</v>
-      </c>
-      <c r="H20" s="10">
-        <v>9.4038828080040505E-15</v>
-      </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="2">
-        <v>24.794</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="18">
-      <c r="A21" s="9" t="s">
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.6077133509280988E-14</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="8">
+        <v>8.4661363426511195E-14</v>
+      </c>
+      <c r="I23" s="8">
+        <f t="shared" si="1"/>
+        <v>-3.9500591546947794E-14</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="2"/>
+        <v>-2.3423458037666807E-14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="18">
+      <c r="A24" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B24" s="8">
         <v>4.8558062973212699E-6</v>
       </c>
-      <c r="C21" s="13">
-        <f t="shared" si="0"/>
-        <v>1.06500622206052E-6</v>
-      </c>
-      <c r="D21" s="10">
+      <c r="C24" s="15"/>
+      <c r="D24" s="8">
         <v>3.7908000752607499E-6</v>
       </c>
-      <c r="E21" s="2">
-        <v>25.785</v>
-      </c>
-      <c r="G21" s="14">
-        <f t="shared" si="1"/>
-        <v>4.4474440992942152E-6</v>
-      </c>
-      <c r="H21" s="10">
-        <v>4.0836219802705499E-7</v>
-      </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="2">
-        <v>24.974</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="18">
-      <c r="A22" s="9" t="s">
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.06500622206052E-6</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="8">
+        <v>4.0836227328453501E-7</v>
+      </c>
+      <c r="I24" s="8">
+        <f t="shared" si="1"/>
+        <v>-4.4474440240367346E-6</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="2"/>
+        <v>-3.382437801976215E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="18">
+      <c r="A25" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B25" s="8">
         <v>1.7570403939339199E-13</v>
       </c>
-      <c r="C22" s="13">
-        <f t="shared" si="0"/>
-        <v>3.8199290033109003E-14</v>
-      </c>
-      <c r="D22" s="10">
+      <c r="C25" s="15"/>
+      <c r="D25" s="8">
         <v>1.3750474936028299E-13</v>
       </c>
-      <c r="E22" s="2">
-        <v>22.216000000000001</v>
-      </c>
-      <c r="G22" s="14">
-        <f t="shared" si="1"/>
-        <v>1.624645571555481E-13</v>
-      </c>
-      <c r="H22" s="10">
-        <v>1.32394822378439E-14</v>
-      </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="2">
-        <v>20.995000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="18">
-      <c r="A23" s="9" t="s">
+      <c r="F25" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.8199290033109003E-14</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="8">
+        <v>1.1194828332593401E-13</v>
+      </c>
+      <c r="I25" s="8">
+        <f t="shared" si="1"/>
+        <v>-6.3755756067457987E-14</v>
+      </c>
+      <c r="K25" s="17">
+        <f t="shared" si="2"/>
+        <v>-2.5556466034348985E-14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="18">
+      <c r="A26" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B26" s="8">
         <v>8.04865641011404E-6</v>
       </c>
-      <c r="C23" s="13">
-        <f t="shared" si="0"/>
-        <v>3.5686199477607902E-6</v>
-      </c>
-      <c r="D23" s="10">
+      <c r="C26" s="15"/>
+      <c r="D26" s="8">
         <v>4.4800364623532498E-6</v>
       </c>
-      <c r="E23" s="2">
-        <v>21.782</v>
-      </c>
-      <c r="G23" s="14">
-        <f t="shared" si="1"/>
-        <v>7.1389188824741962E-6</v>
-      </c>
-      <c r="H23" s="10">
-        <v>9.0973752763984405E-7</v>
-      </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="2">
-        <v>21.033000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="18">
-      <c r="A24" s="9" t="s">
+      <c r="F26" s="8">
+        <f t="shared" si="0"/>
+        <v>-3.5686199477607902E-6</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="8">
+        <v>9.0973762634864496E-7</v>
+      </c>
+      <c r="I26" s="8">
+        <f t="shared" si="1"/>
+        <v>-7.1389187837653947E-6</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" si="2"/>
+        <v>-3.5702988360046048E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="18">
+      <c r="A27" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B27" s="8">
         <v>8.4992513937415601E-14</v>
       </c>
-      <c r="C24" s="13">
-        <f t="shared" si="0"/>
-        <v>1.5960390502916707E-14</v>
-      </c>
-      <c r="D24" s="10">
+      <c r="C27" s="15"/>
+      <c r="D27" s="8">
         <v>6.9032123434498894E-14</v>
       </c>
-      <c r="E24" s="2">
-        <v>24.875</v>
-      </c>
-      <c r="G24" s="14">
-        <f t="shared" si="1"/>
-        <v>7.5543013074638276E-14</v>
-      </c>
-      <c r="H24" s="10">
-        <v>9.4495008627773206E-15</v>
-      </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="2">
-        <v>24.042999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="18">
-      <c r="A25" s="9" t="s">
+      <c r="F27" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.5960390502916707E-14</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="8">
+        <v>6.1238980620744505E-14</v>
+      </c>
+      <c r="I27" s="8">
+        <f t="shared" si="1"/>
+        <v>-2.3753533316671096E-14</v>
+      </c>
+      <c r="K27" s="17">
+        <f t="shared" si="2"/>
+        <v>-7.7931428137543892E-15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="18">
+      <c r="A28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B28" s="8">
         <v>3.3491639257841102E-6</v>
       </c>
-      <c r="C25" s="13">
-        <f t="shared" si="0"/>
-        <v>1.3580366012635904E-6</v>
-      </c>
-      <c r="D25" s="10">
+      <c r="C28" s="15"/>
+      <c r="D28" s="8">
         <v>1.9911273245205198E-6</v>
       </c>
-      <c r="E25" s="2">
-        <v>24.954000000000001</v>
-      </c>
-      <c r="G25" s="14">
-        <f t="shared" si="1"/>
-        <v>2.2325851790292702E-6</v>
-      </c>
-      <c r="H25" s="10">
-        <v>1.11657874675484E-6</v>
-      </c>
-      <c r="I25" s="10"/>
-      <c r="J25" s="2">
-        <v>24.478999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="18">
-      <c r="A26" s="9" t="s">
+      <c r="F28" s="8">
+        <f t="shared" si="0"/>
+        <v>-1.3580366012635904E-6</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="8">
+        <v>1.1165787985443201E-6</v>
+      </c>
+      <c r="I28" s="8">
+        <f t="shared" si="1"/>
+        <v>-2.2325851272397903E-6</v>
+      </c>
+      <c r="K28" s="17">
+        <f t="shared" si="2"/>
+        <v>-8.7454852597619976E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="18">
+      <c r="A29" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B29" s="8">
         <v>6.8178507059484301E-16</v>
       </c>
-      <c r="C26" s="12">
-        <f t="shared" si="0"/>
-        <v>-1.2302432823460671E-15</v>
-      </c>
-      <c r="D26" s="10">
+      <c r="C29" s="15"/>
+      <c r="D29" s="8">
         <v>1.9120283529409101E-15</v>
       </c>
-      <c r="E26" s="2">
-        <v>16.794</v>
-      </c>
-      <c r="G26" s="14">
-        <f t="shared" si="1"/>
-        <v>3.9695041899877803E-16</v>
-      </c>
-      <c r="H26" s="10">
-        <v>2.8483465159606498E-16</v>
-      </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="2">
-        <v>14.877000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="18">
-      <c r="A27" s="9" t="s">
+      <c r="F29" s="8">
+        <f t="shared" si="0"/>
+        <v>1.2302432823460671E-15</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="8">
+        <v>7.01986109635643E-16</v>
+      </c>
+      <c r="I29" s="16">
+        <f t="shared" si="1"/>
+        <v>2.0201039040799988E-17</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.2100422433052671E-15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="18">
+      <c r="A30" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B30" s="2">
         <v>2.81033459978085E-4</v>
       </c>
-      <c r="C27" s="12">
-        <f t="shared" si="0"/>
-        <v>-3.0851300534435449E-3</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C30" s="15"/>
+      <c r="D30" s="2">
         <v>3.36616351342163E-3</v>
       </c>
-      <c r="E27" s="2">
-        <v>16.838999999999999</v>
-      </c>
-      <c r="G27" s="15">
-        <f t="shared" si="1"/>
-        <v>-4.5486859672212016E-5</v>
-      </c>
-      <c r="H27" s="2">
-        <v>3.2652031965029702E-4</v>
-      </c>
-      <c r="J27" s="2">
-        <v>16.591999999999999</v>
+      <c r="F30" s="8">
+        <f t="shared" si="0"/>
+        <v>3.0851300534435449E-3</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="2">
+        <v>3.26520319650714E-4</v>
+      </c>
+      <c r="I30" s="16">
+        <f t="shared" si="1"/>
+        <v>4.5486859672629E-5</v>
+      </c>
+      <c r="K30" s="17">
+        <f t="shared" si="2"/>
+        <v>-3.0396431937709158E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D2:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="C4:C27">
+  <conditionalFormatting sqref="C4:C30">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>"&lt;0.0"</formula>
     </cfRule>

</xml_diff>

<commit_message>
val and loop experiments
</commit_message>
<xml_diff>
--- a/graphs/lipschitz_results.xlsx
+++ b/graphs/lipschitz_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28720" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Loops" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="146">
   <si>
     <t>Jet Engine</t>
   </si>
@@ -305,12 +305,6 @@
     <t>Benchmark name</t>
   </si>
   <si>
-    <t>loop bound</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spiral </t>
-  </si>
-  <si>
     <t>Harmonic oscillator</t>
   </si>
   <si>
@@ -335,30 +329,6 @@
     <t>unrolled error</t>
   </si>
   <si>
-    <t>error infinity norm</t>
-  </si>
-  <si>
-    <t>error componentwise</t>
-  </si>
-  <si>
-    <t>unrolling time</t>
-  </si>
-  <si>
-    <t>lipschitz time</t>
-  </si>
-  <si>
-    <t>  1.7270990036681887e-14</t>
-  </si>
-  <si>
-    <t>   2.150892019569794e-14</t>
-  </si>
-  <si>
-    <t>            2.0873007675817594e-14</t>
-  </si>
-  <si>
-    <t>            2.5640677248553363e-13</t>
-  </si>
-  <si>
     <t>euler  x</t>
   </si>
   <si>
@@ -377,9 +347,6 @@
     <t>without energy bound</t>
   </si>
   <si>
-    <t>with energy bound</t>
-  </si>
-  <si>
     <t>Mean/Variance</t>
   </si>
   <si>
@@ -389,20 +356,126 @@
     <t>variance</t>
   </si>
   <si>
-    <t>Infinity</t>
-  </si>
-  <si>
     <t>p1 norm</t>
   </si>
   <si>
     <t>p2 norm</t>
+  </si>
+  <si>
+    <t>error Lipschitz</t>
+  </si>
+  <si>
+    <t>time for Lipschitz</t>
+  </si>
+  <si>
+    <t>Harmonic oscillator (with energy bound)</t>
+  </si>
+  <si>
+    <t>Spiral (50 loops)</t>
+  </si>
+  <si>
+    <t>euler v</t>
+  </si>
+  <si>
+    <t>rk2 v</t>
+  </si>
+  <si>
+    <t>rk2 x</t>
+  </si>
+  <si>
+    <t>rk4 x</t>
+  </si>
+  <si>
+    <t>rk4 v</t>
+  </si>
+  <si>
+    <t>Pendulum (10 iterations)</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>omega</t>
+  </si>
+  <si>
+    <t>time for unrolling (~in s)</t>
+  </si>
+  <si>
+    <t>Without Lipschitz at all - With Lipschitz and with vals - straightline with lipschitz</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>without Lipschitz</t>
+  </si>
+  <si>
+    <t>with Lipschitz and vals</t>
+  </si>
+  <si>
+    <t>straightline with Lipschitz</t>
+  </si>
+  <si>
+    <t> 3.8995993844220517e-13</t>
+  </si>
+  <si>
+    <t> in</t>
+  </si>
+  <si>
+    <t>jetEngine1</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>jetEngine1_2</t>
+  </si>
+  <si>
+    <t>jetEngine2</t>
+  </si>
+  <si>
+    <t>jetEngine2_2</t>
+  </si>
+  <si>
+    <t>predatorPrey2</t>
+  </si>
+  <si>
+    <t>rigidBody1_2</t>
+  </si>
+  <si>
+    <t>rigidBody2_2</t>
+  </si>
+  <si>
+    <t>in (cummulative)</t>
+  </si>
+  <si>
+    <t>turbine1 - 1</t>
+  </si>
+  <si>
+    <t>turbine1 - 2</t>
+  </si>
+  <si>
+    <t>turbine1 - 3</t>
+  </si>
+  <si>
+    <t>turbine2 -1</t>
+  </si>
+  <si>
+    <t>turbine2 - 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turbine2 - 3 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -470,13 +543,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,6 +581,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -505,7 +597,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -591,8 +683,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -642,24 +766,25 @@
     <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -669,8 +794,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -713,6 +860,22 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -755,6 +918,22 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1095,417 +1274,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J48"/>
+  <dimension ref="A3:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="27" style="31" customWidth="1"/>
+    <col min="4" max="4" width="20.5" style="35" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="33" customWidth="1"/>
     <col min="6" max="6" width="26.83203125" style="16" customWidth="1"/>
     <col min="7" max="7" width="24.1640625" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="31">
+        <v>1.56449911370704E-12</v>
+      </c>
+      <c r="C4" s="31">
+        <v>3.7656645169696701E-12</v>
+      </c>
+      <c r="D4" s="35">
+        <v>500</v>
+      </c>
+      <c r="E4" s="33">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="31">
+        <v>9.6819412127175898E-15</v>
+      </c>
+      <c r="C7" s="31">
+        <v>8.9664264371202206E-15</v>
+      </c>
+      <c r="D7" s="35">
+        <v>6550</v>
+      </c>
+      <c r="E7" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="31">
+        <v>2.7413533889205399E-14</v>
+      </c>
+      <c r="C8" s="31">
+        <v>9.1618720783776298E-15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="I3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" t="s">
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="15" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2.0409942805719001E-14</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="6"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="26" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="31">
+        <v>2.7025936423277E-14</v>
+      </c>
+      <c r="C12" s="31">
+        <v>5.1659130607197298E-14</v>
+      </c>
+      <c r="D12" s="35">
+        <v>14</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2.7025936423277E-14</v>
-      </c>
-      <c r="E8" s="17">
-        <v>1.11022302462515E-15</v>
-      </c>
-      <c r="F8" s="17">
-        <v>2.9091550168460802E-14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="B13" s="31">
         <v>4.1521637247621297E-14</v>
       </c>
-      <c r="E9" s="17">
-        <v>1.11022302462515E-15</v>
-      </c>
-      <c r="F9" s="17">
-        <v>4.1882844374033703E-14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="6"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C13" s="31">
+        <v>7.3519540407003096E-14</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6"/>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="31">
         <v>4.5343376285040698E-14</v>
       </c>
-      <c r="E11" s="17">
-        <v>1.5182471257219901E-14</v>
-      </c>
-      <c r="F11" s="17">
-        <v>3.1977537851133303E-14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C15" s="31">
+        <v>5.3108496003304797E-14</v>
+      </c>
+      <c r="D15" s="35">
+        <v>118</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0.7</v>
+      </c>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="31">
         <v>6.7865302772859896E-14</v>
       </c>
-      <c r="E12" s="17">
-        <v>2.1720346053341599E-14</v>
-      </c>
-      <c r="F12" s="17">
-        <v>4.7973597328009297E-14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="6"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" s="1">
-        <v>8.5984594476302397E-14</v>
-      </c>
-      <c r="E14" s="17">
-        <v>2.0445916583857499E-14</v>
-      </c>
-      <c r="F14" s="17">
-        <v>4.4272881658956601E-14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1.4094190022924499E-13</v>
-      </c>
-      <c r="E15" s="17">
-        <v>3.3150000264270299E-14</v>
-      </c>
-      <c r="F15" s="17">
-        <v>6.8472625751640502E-14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="6"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="17"/>
+      <c r="C16" s="31">
+        <v>7.75741744648248E-14</v>
+      </c>
       <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
+      <c r="A17" s="6"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2.38219847429337E-14</v>
-      </c>
-      <c r="E18" s="17">
-        <v>1.11022302462515E-15</v>
-      </c>
-      <c r="F18" s="17">
-        <v>2.75071328989052E-14</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B18" s="31">
+        <v>8.0143306021600802E-14</v>
+      </c>
+      <c r="C18" s="31">
+        <v>6.5341011774180005E-14</v>
+      </c>
+      <c r="D18" s="35">
+        <v>510</v>
+      </c>
+      <c r="E18" s="33">
+        <v>9</v>
+      </c>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="1">
-        <v>3.6431649253377398E-14</v>
-      </c>
-      <c r="E19" s="17">
-        <v>1.11022302462515E-15</v>
-      </c>
-      <c r="F19" s="17">
-        <v>3.9936183843700702E-14</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="B19" s="31">
+        <v>1.2350085764037499E-13</v>
+      </c>
+      <c r="C19" s="31">
+        <v>9.7970669332456603E-14</v>
+      </c>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="6"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="17"/>
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="1">
-        <v>3.97986659514232E-14</v>
-      </c>
-      <c r="E21" s="17">
-        <v>1.41897449894784E-14</v>
-      </c>
-      <c r="F21" s="17">
-        <v>2.9028749466235199E-14</v>
-      </c>
+      <c r="A21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="1">
-        <v>5.9900906518422805E-14</v>
-      </c>
-      <c r="E22" s="17">
-        <v>2.0775486811862599E-14</v>
-      </c>
-      <c r="F22" s="17">
-        <v>4.2497221193815202E-14</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="6"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="1">
-        <v>7.9793557854425903E-14</v>
-      </c>
-      <c r="E24" s="17">
-        <v>1.91856734776144E-14</v>
-      </c>
-      <c r="F24" s="17">
-        <v>4.4895949915819201E-14</v>
-      </c>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1.30701626033781E-13</v>
-      </c>
-      <c r="E25" s="17">
-        <v>3.7702118809566702E-14</v>
-      </c>
-      <c r="F25" s="17">
-        <v>7.2893255206989901E-14</v>
-      </c>
+      <c r="A25" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="6"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="17"/>
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
       <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="15" t="s">
+      <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6"/>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="6" t="s">
+    <row r="32" spans="1:6">
+      <c r="A32" s="6"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="15" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="6"/>
-    </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="6"/>
+      <c r="A34" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="15" t="s">
-        <v>46</v>
+      <c r="A35" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="6"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="6"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40">
-        <v>1000</v>
-      </c>
-      <c r="E40" s="17">
-        <v>1.26562932716027E-7</v>
-      </c>
-      <c r="F40" s="17">
-        <v>1.2650419745343501E-7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>119</v>
-      </c>
-      <c r="B41">
-        <v>1000</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="F41" s="16">
-        <v>0.13270591776410801</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="18">
-      <c r="A45" s="7"/>
-    </row>
-    <row r="46" spans="1:6" ht="18">
-      <c r="A46" s="7"/>
-    </row>
-    <row r="47" spans="1:6" ht="18">
-      <c r="A47" s="7"/>
-    </row>
-    <row r="48" spans="1:6" ht="18">
-      <c r="A48" s="7"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="6"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="6"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A17:F17"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1518,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P60"/>
+  <dimension ref="A2:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1542,10 +1649,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16">
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="27"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:16" ht="30">
       <c r="A3" s="2" t="s">
@@ -2382,12 +2489,12 @@
         <v>55</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="23" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2401,10 +2508,10 @@
       <c r="C34" s="8">
         <v>2.4391675624488901E-8</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="24">
         <v>2.25750855333976E-8</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="23">
         <v>291.82212204267501</v>
       </c>
     </row>
@@ -2418,10 +2525,10 @@
       <c r="C35" s="2">
         <v>176542.39050431299</v>
       </c>
-      <c r="D35" s="23">
+      <c r="D35" s="25">
         <v>168548.397053803</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="23">
         <v>375500000000</v>
       </c>
     </row>
@@ -2435,10 +2542,10 @@
       <c r="C36" s="8">
         <v>4.8247373575872301E-13</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="24">
         <v>4.66355777193661E-13</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="26">
         <v>7.5687712674192001E-12</v>
       </c>
     </row>
@@ -2452,10 +2559,10 @@
       <c r="C37" s="8">
         <v>1.0773840322254299E-6</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D37" s="24">
         <v>8.2134348581501601E-7</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="26">
         <v>3.2162376167005601E-6</v>
       </c>
     </row>
@@ -2469,10 +2576,10 @@
       <c r="C38" s="8">
         <v>1.2582571520286501E-12</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="24">
         <v>1.2239270289057101E-12</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="26">
         <v>2.3788848349489198E-11</v>
       </c>
     </row>
@@ -2486,10 +2593,10 @@
       <c r="C39" s="8">
         <v>2.7532011678784899E-5</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="24">
         <v>2.0493458540005501E-5</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="23">
         <v>8.1719907176002193E-3</v>
       </c>
     </row>
@@ -2503,10 +2610,10 @@
       <c r="C40" s="8">
         <v>1.89817199412561E-13</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="24">
         <v>1.8368072731251901E-13</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40" s="26">
         <v>1.5508963403060401E-12</v>
       </c>
     </row>
@@ -2520,7 +2627,7 @@
       <c r="C41" s="8">
         <v>6.1253569445074093E-5</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="24">
         <v>6.1212462342366902E-5</v>
       </c>
       <c r="E41" s="24">
@@ -2537,10 +2644,10 @@
       <c r="C42" s="8">
         <v>8.4020009457044304E-9</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="24">
         <v>8.4014068474587507E-9</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="26">
         <v>8.5601678323450507E-9</v>
       </c>
     </row>
@@ -2554,7 +2661,7 @@
       <c r="C43" s="2">
         <v>9.5604725233654599E-4</v>
       </c>
-      <c r="D43" s="23">
+      <c r="D43" s="25">
         <v>9.5336028036743304E-4</v>
       </c>
       <c r="E43" s="25">
@@ -2571,10 +2678,10 @@
       <c r="C44" s="8">
         <v>2.9395681973922702E-16</v>
       </c>
-      <c r="D44" s="22">
+      <c r="D44" s="24">
         <v>2.5680196768409301E-16</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="26">
         <v>1.2160792721113199E-15</v>
       </c>
     </row>
@@ -2582,16 +2689,16 @@
       <c r="A45" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="24">
+      <c r="B45" s="21">
         <v>9.21678116374064E-5</v>
       </c>
       <c r="C45" s="8">
         <v>9.7853112216226301E-5</v>
       </c>
-      <c r="D45" s="21">
+      <c r="D45" s="26">
         <v>9.5055869548972598E-5</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="23">
         <v>2.3615113285604598E-3</v>
       </c>
     </row>
@@ -2605,7 +2712,7 @@
       <c r="C46" s="8">
         <v>5.07927054883157E-13</v>
       </c>
-      <c r="D46" s="21">
+      <c r="D46" s="26">
         <v>4.4953803356846002E-13</v>
       </c>
       <c r="E46" s="24">
@@ -2622,7 +2729,7 @@
       <c r="C47" s="8">
         <v>9.2000035471627699E-7</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="26">
         <v>5.6938598853574696E-7</v>
       </c>
       <c r="E47" s="24">
@@ -2639,7 +2746,7 @@
       <c r="C48" s="8">
         <v>6.4751830231218804E-11</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="26">
         <v>5.4848635250135298E-11</v>
       </c>
       <c r="E48" s="24">
@@ -2656,7 +2763,7 @@
       <c r="C49" s="2">
         <v>1.5031003972018601E-4</v>
       </c>
-      <c r="D49" s="21">
+      <c r="D49" s="26">
         <v>9.0843339418073099E-5</v>
       </c>
       <c r="E49" s="24">
@@ -2670,10 +2777,10 @@
       <c r="B50" s="8">
         <v>9.5541167016934297E-16</v>
       </c>
-      <c r="C50" s="24">
+      <c r="C50" s="21">
         <v>7.6462185813549397E-16</v>
       </c>
-      <c r="D50" s="22">
+      <c r="D50" s="24">
         <v>7.6462185813549397E-16</v>
       </c>
       <c r="E50" s="24">
@@ -2687,10 +2794,10 @@
       <c r="B51" s="8">
         <v>1.1079985983775101E-15</v>
       </c>
-      <c r="C51" s="24">
+      <c r="C51" s="21">
         <v>8.7883766303940201E-16</v>
       </c>
-      <c r="D51" s="22">
+      <c r="D51" s="24">
         <v>8.7883766303940201E-16</v>
       </c>
       <c r="E51" s="24">
@@ -2704,10 +2811,10 @@
       <c r="B52" s="8">
         <v>8.4047352454551996E-16</v>
       </c>
-      <c r="C52" s="24">
+      <c r="C52" s="21">
         <v>8.1098322541998701E-16</v>
       </c>
-      <c r="D52" s="22">
+      <c r="D52" s="24">
         <v>8.1098322541998701E-16</v>
       </c>
       <c r="E52" s="24">
@@ -2724,10 +2831,10 @@
       <c r="C53" s="8">
         <v>8.4661363426511195E-14</v>
       </c>
-      <c r="D53" s="22">
+      <c r="D53" s="24">
         <v>8.0920161324566205E-14</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="26">
         <v>1.08084821464178E-13</v>
       </c>
     </row>
@@ -2741,10 +2848,10 @@
       <c r="C54" s="8">
         <v>4.0836227328453501E-7</v>
       </c>
-      <c r="D54" s="22">
+      <c r="D54" s="24">
         <v>3.67125149087156E-7</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="26">
         <v>3.7908000752607499E-6</v>
       </c>
     </row>
@@ -2758,10 +2865,10 @@
       <c r="C55" s="8">
         <v>1.1194828332593401E-13</v>
       </c>
-      <c r="D55" s="22">
+      <c r="D55" s="24">
         <v>1.0635419190329001E-13</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E55" s="26">
         <v>1.3750474936028299E-13</v>
       </c>
     </row>
@@ -2775,10 +2882,10 @@
       <c r="C56" s="8">
         <v>9.0973762634864496E-7</v>
       </c>
-      <c r="D56" s="22">
+      <c r="D56" s="24">
         <v>8.5955587936852099E-7</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E56" s="26">
         <v>4.4800364623532498E-6</v>
       </c>
     </row>
@@ -2792,10 +2899,10 @@
       <c r="C57" s="8">
         <v>6.1238980620744505E-14</v>
       </c>
-      <c r="D57" s="22">
+      <c r="D57" s="24">
         <v>5.7936950132578094E-14</v>
       </c>
-      <c r="E57" s="8">
+      <c r="E57" s="26">
         <v>6.9032123434498894E-14</v>
       </c>
     </row>
@@ -2809,10 +2916,10 @@
       <c r="C58" s="8">
         <v>1.1165787985443201E-6</v>
       </c>
-      <c r="D58" s="22">
+      <c r="D58" s="24">
         <v>1.0937431479027001E-6</v>
       </c>
-      <c r="E58" s="8">
+      <c r="E58" s="26">
         <v>1.9911273245205198E-6</v>
       </c>
     </row>
@@ -2826,10 +2933,10 @@
       <c r="C59" s="8">
         <v>7.01986109635643E-16</v>
       </c>
-      <c r="D59" s="22">
+      <c r="D59" s="24">
         <v>6.00919856798164E-16</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E59" s="26">
         <v>1.9120283529409101E-15</v>
       </c>
     </row>
@@ -2837,18 +2944,511 @@
       <c r="A60" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B60" s="25">
+      <c r="B60" s="22">
         <v>2.81033459978085E-4</v>
       </c>
       <c r="C60" s="2">
         <v>3.26520319650714E-4</v>
       </c>
-      <c r="D60" s="19">
+      <c r="D60" s="23">
         <v>3.20722399236392E-4</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="23">
         <v>3.36616351342163E-3</v>
       </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="E66" s="37"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="E67" s="37"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="38"/>
+      <c r="B68" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E68" s="37"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" s="39">
+        <v>4.91905140346289E-13</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="36">
+        <v>4.9406853531697201E-13</v>
+      </c>
+      <c r="E69" s="37"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="37">
+        <v>6.24</v>
+      </c>
+      <c r="C70" s="37">
+        <v>39.253999999999998</v>
+      </c>
+      <c r="D70" s="19">
+        <v>44.887999999999998</v>
+      </c>
+      <c r="E70" s="37"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B71" s="39">
+        <v>1.61703982148642E-8</v>
+      </c>
+      <c r="C71" s="39">
+        <v>7.9937127221194098E-9</v>
+      </c>
+      <c r="D71" s="36">
+        <v>8.4030267871834596E-9</v>
+      </c>
+      <c r="E71" s="37"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B72" s="37">
+        <v>120.10899999999999</v>
+      </c>
+      <c r="C72" s="37">
+        <v>705.54</v>
+      </c>
+      <c r="D72" s="19">
+        <v>812.29499999999996</v>
+      </c>
+      <c r="E72" s="37"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="37">
+        <v>0.14001733998549501</v>
+      </c>
+      <c r="C73" s="37">
+        <v>4.2866564318308599E-3</v>
+      </c>
+      <c r="D73" s="19">
+        <v>9.5726361715936395E-4</v>
+      </c>
+      <c r="E73" s="37"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B74" s="37">
+        <v>120.67</v>
+      </c>
+      <c r="C74" s="37">
+        <v>677.28899999999999</v>
+      </c>
+      <c r="D74" s="19">
+        <v>903.29300000000001</v>
+      </c>
+      <c r="E74" s="37"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B75" s="39">
+        <v>1.6157651619324299E-8</v>
+      </c>
+      <c r="C75" s="39">
+        <v>1.2674466936664101E-8</v>
+      </c>
+      <c r="D75" s="36">
+        <v>8.4030267871834596E-9</v>
+      </c>
+      <c r="E75" s="37"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="37">
+        <v>119.06100000000001</v>
+      </c>
+      <c r="C76" s="37">
+        <v>312.709</v>
+      </c>
+      <c r="D76" s="19">
+        <v>812.29499999999996</v>
+      </c>
+      <c r="E76" s="37"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="B77" s="37">
+        <v>0.13990366557440501</v>
+      </c>
+      <c r="C77" s="37">
+        <v>0.111173717124204</v>
+      </c>
+      <c r="D77" s="19">
+        <v>9.5726361715936395E-4</v>
+      </c>
+      <c r="E77" s="37"/>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B78" s="37">
+        <v>119.602</v>
+      </c>
+      <c r="C78" s="37">
+        <v>353.702</v>
+      </c>
+      <c r="D78" s="19">
+        <v>903.29300000000001</v>
+      </c>
+      <c r="E78" s="37"/>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" s="39">
+        <v>2.93531236761047E-16</v>
+      </c>
+      <c r="C79" s="39">
+        <v>9.2296026520911794E-5</v>
+      </c>
+      <c r="D79" s="36">
+        <v>2.9395681979020301E-16</v>
+      </c>
+      <c r="E79" s="37"/>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B80" s="37">
+        <v>3.5579999999999998</v>
+      </c>
+      <c r="C80" s="37">
+        <v>24.459</v>
+      </c>
+      <c r="D80" s="19">
+        <v>63.177</v>
+      </c>
+      <c r="E80" s="37"/>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B81" s="39">
+        <v>9.21678116374064E-5</v>
+      </c>
+      <c r="C81" s="39">
+        <v>9.2296026520911794E-5</v>
+      </c>
+      <c r="D81" s="36">
+        <v>9.7854698929362996E-5</v>
+      </c>
+      <c r="E81" s="37"/>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B82" s="37">
+        <v>3.5409999999999999</v>
+      </c>
+      <c r="C82" s="37">
+        <v>29.074000000000002</v>
+      </c>
+      <c r="D82" s="19">
+        <v>61.851999999999997</v>
+      </c>
+      <c r="E82" s="37"/>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="39">
+        <v>5.0792705700022197E-13</v>
+      </c>
+      <c r="C83" s="39">
+        <v>5.07927051422957E-13</v>
+      </c>
+      <c r="D83" s="36">
+        <v>5.07927054883157E-13</v>
+      </c>
+      <c r="E83" s="37"/>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B84" s="37">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C84" s="37">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="D84" s="19">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="E84" s="37"/>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="B85" s="39">
+        <v>9.2000035501627902E-7</v>
+      </c>
+      <c r="C85" s="39">
+        <v>9.2000035531627405E-7</v>
+      </c>
+      <c r="D85" s="36">
+        <v>9.2000035531627702E-7</v>
+      </c>
+      <c r="E85" s="37"/>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B86" s="37">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C86" s="37">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="D86" s="19">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="E86" s="37"/>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="39">
+        <v>6.4751831136229797E-11</v>
+      </c>
+      <c r="C87" s="39">
+        <v>6.4751771931891497E-11</v>
+      </c>
+      <c r="D87" s="36">
+        <v>6.4751830624155806E-11</v>
+      </c>
+      <c r="E87" s="37"/>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B88" s="37">
+        <v>6.3769999999999998</v>
+      </c>
+      <c r="C88" s="37">
+        <v>6.9109999999999996</v>
+      </c>
+      <c r="D88" s="19">
+        <v>7.4889999999999999</v>
+      </c>
+      <c r="E88" s="37"/>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="B89" s="37">
+        <v>1.50310039864787E-4</v>
+      </c>
+      <c r="C89" s="37">
+        <v>1.5031004000932801E-4</v>
+      </c>
+      <c r="D89" s="19">
+        <v>1.5031004000938699E-4</v>
+      </c>
+      <c r="E89" s="37"/>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B90" s="37">
+        <v>6.4119999999999999</v>
+      </c>
+      <c r="C90" s="37">
+        <v>6.9089999999999998</v>
+      </c>
+      <c r="D90" s="19">
+        <v>7.5880000000000001</v>
+      </c>
+      <c r="E90" s="37"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="B91" s="36">
+        <v>1.2416195497345899E-13</v>
+      </c>
+      <c r="C91" s="39">
+        <v>7.1459995549231998E-14</v>
+      </c>
+      <c r="D91" s="39">
+        <v>8.46613634280406E-14</v>
+      </c>
+      <c r="E91" s="37"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" s="36">
+        <v>1.7570403939339199E-13</v>
+      </c>
+      <c r="C92" s="39">
+        <v>9.0254690823196797E-14</v>
+      </c>
+      <c r="D92" s="39">
+        <v>1.11948283327741E-13</v>
+      </c>
+      <c r="E92" s="37"/>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="36">
+        <v>8.4992513937415601E-14</v>
+      </c>
+      <c r="C93" s="39">
+        <v>5.1653211495252003E-14</v>
+      </c>
+      <c r="D93" s="39">
+        <v>6.1238980621548095E-14</v>
+      </c>
+      <c r="E93" s="37"/>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" s="37">
+        <v>14.391</v>
+      </c>
+      <c r="C94" s="37">
+        <v>33.54</v>
+      </c>
+      <c r="D94" s="19">
+        <v>87.962999999999994</v>
+      </c>
+      <c r="E94" s="37"/>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B95" s="36">
+        <v>4.8558062973212699E-6</v>
+      </c>
+      <c r="C95" s="39">
+        <v>4.0900699725744698E-7</v>
+      </c>
+      <c r="D95" s="39">
+        <v>4.0836233128749301E-7</v>
+      </c>
+      <c r="E95" s="37"/>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="B96" s="36">
+        <v>8.04865641011404E-6</v>
+      </c>
+      <c r="C96" s="39">
+        <v>9.0973783297971903E-7</v>
+      </c>
+      <c r="D96" s="39">
+        <v>9.0973785467089302E-7</v>
+      </c>
+      <c r="E96" s="37"/>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="B97" s="36">
+        <v>3.3491639257841102E-6</v>
+      </c>
+      <c r="C97" s="39">
+        <v>1.11722363934565E-6</v>
+      </c>
+      <c r="D97" s="39">
+        <v>1.11657896976839E-6</v>
+      </c>
+      <c r="E97" s="37"/>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B98" s="37">
+        <v>14.478999999999999</v>
+      </c>
+      <c r="C98" s="37">
+        <v>34.389000000000003</v>
+      </c>
+      <c r="D98" s="19">
+        <v>89.322000000000003</v>
+      </c>
+      <c r="E98" s="37"/>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="37"/>
+      <c r="B99" s="37"/>
+      <c r="C99" s="37"/>
+      <c r="E99" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3037,16 +3637,16 @@
   <sheetData>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="18">
       <c r="A2" s="5"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="J2" s="28" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="J2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="28"/>
+      <c r="K2" s="29"/>
       <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="36">

</xml_diff>